<commit_message>
Atualizando critério de inovação
</commit_message>
<xml_diff>
--- a/Excel/Critério de inovação.xlsx
+++ b/Excel/Critério de inovação.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\Documentos\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A47ABC-C2CD-4276-A1C8-92CBD479F89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E54B83-F925-4730-87F7-5F3BC43BBBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,18 +170,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -359,78 +353,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2893,15 +2885,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:colOff>236220</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:colOff>640080</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2931,7 +2923,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2842260" y="2910840"/>
+          <a:off x="2834640" y="2628900"/>
           <a:ext cx="403860" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4212,7 +4204,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2827020" y="3177540"/>
+          <a:off x="2827020" y="2994660"/>
           <a:ext cx="403860" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6248,15 +6240,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
+      <xdr:colOff>632460</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6286,7 +6278,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6568440" y="1920240"/>
+          <a:off x="6576060" y="1905000"/>
           <a:ext cx="403860" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6553,15 +6545,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
+      <xdr:colOff>335280</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>525780</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6591,7 +6583,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6659880" y="2362200"/>
+          <a:off x="6682740" y="2369820"/>
           <a:ext cx="190500" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6858,13 +6850,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
+      <xdr:colOff>243840</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
@@ -6896,7 +6888,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6553200" y="2438400"/>
+          <a:off x="6591300" y="2438400"/>
           <a:ext cx="403860" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6980,13 +6972,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:colOff>251460</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
+      <xdr:colOff>655320</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
@@ -7018,7 +7010,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6560820" y="2621280"/>
+          <a:off x="6598920" y="2621280"/>
           <a:ext cx="403860" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7163,15 +7155,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:colOff>236220</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
+      <xdr:colOff>640080</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7201,7 +7193,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6560820" y="2819400"/>
+          <a:off x="6583680" y="2811780"/>
           <a:ext cx="403860" cy="403860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7224,13 +7216,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>327660</xdr:colOff>
+      <xdr:colOff>350520</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:colOff>541020</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
@@ -7262,7 +7254,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6675120" y="3116580"/>
+          <a:off x="6697980" y="3116580"/>
           <a:ext cx="190500" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7768,7 +7760,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7785,263 +7777,264 @@
         <v>0</v>
       </c>
       <c r="B1" s="19"/>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="20" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="9"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="2"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="8"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="1"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="5"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="5"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="15"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="5"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="3"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="5"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="10"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="1"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A12:B12"/>
@@ -8058,7 +8051,6 @@
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>